<commit_message>
@debv push 0908 win
</commit_message>
<xml_diff>
--- a/201709资源商城迭代/windows/9月课程中心迭代 - 技术开发量 粗估（后端）.xlsx
+++ b/201709资源商城迭代/windows/9月课程中心迭代 - 技术开发量 粗估（后端）.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -456,15 +456,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（0.5）运营后台-创建企业站点
-（1）企业站点列表 + 企业站点查看资料
-     （索引增加类型 + 搜索接口 + 列表增加列显示）
-（1）方法注解设计实现 
-（1.5）用户访受限看视频的提示
-     （并发数redis实现 + 检测接口 + 范围排查）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">
 （0.5）授课方式 + 授课时间 + 列表兼容性考虑
 </t>
@@ -478,11 +469,6 @@
   <si>
     <t>课程中心-机构后台
 （0.5+4.5+3+1 =9）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>“并发访问人数”销售
-     （4）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -523,7 +509,7 @@
   <si>
     <r>
       <t>【备注】：该评估仅为粗估，,仅作为策划拆分迭代节奏的参考，不作为实际迭代排期WBS，实际WBS需要开发模块设计评审之后才能做到更精准的估算。
-【后端】：开发（含自测，22.5+4） + 联调（2*3）+ 冒烟（3*3） = 41.5
+【后端】：开发（含自测，22.5） + 联调（2*3）+ 冒烟（3*3） = 37.5
 【</t>
     </r>
     <r>
@@ -608,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,12 +634,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4BD0FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3300"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,7 +758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -928,21 +908,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1268,7 +1233,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I337"/>
+  <dimension ref="A1:I336"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1288,7 +1253,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1376,7 +1341,7 @@
         <v>68</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>4</v>
@@ -1396,7 +1361,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>4</v>
@@ -1416,7 +1381,7 @@
         <v>70</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>4</v>
@@ -1432,7 +1397,7 @@
     </row>
     <row r="9" spans="1:9" ht="108" x14ac:dyDescent="0.15">
       <c r="A9" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="26" t="s">
@@ -1453,13 +1418,13 @@
     </row>
     <row r="10" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A10" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>74</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>4</v>
@@ -1537,80 +1502,72 @@
       </c>
       <c r="I13" s="36"/>
     </row>
-    <row r="14" spans="1:9" ht="81" x14ac:dyDescent="0.15">
-      <c r="A14" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="53">
-        <v>4</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="12"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
+      <c r="A15" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="14"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="14"/>
       <c r="G16" s="19"/>
       <c r="H16" s="14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+      <c r="A17" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="17"/>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="14"/>
       <c r="G17" s="19"/>
       <c r="H17" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="27" x14ac:dyDescent="0.15">
-      <c r="A18" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="14">
-        <f>SUM(H4:H17)</f>
-        <v>41.5</v>
-      </c>
+        <f>SUM(H4:H16)</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C19" s="5"/>
@@ -1653,14 +1610,12 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="C25" s="5"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -1702,7 +1657,6 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="C32" s="5"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -3226,11 +3180,6 @@
       <c r="F336" s="8"/>
       <c r="G336" s="8"/>
       <c r="H336" s="8"/>
-    </row>
-    <row r="337" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F337" s="8"/>
-      <c r="G337" s="8"/>
-      <c r="H337" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>